<commit_message>
added sample DB structure
</commit_message>
<xml_diff>
--- a/sampleTWDB.xlsx
+++ b/sampleTWDB.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzhenko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,29 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>VendorID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Product Name</t>
   </si>
   <si>
-    <t>MeasureID</t>
-  </si>
-  <si>
-    <t>Base Price</t>
-  </si>
-  <si>
     <t>Sword alabala</t>
   </si>
   <si>
-    <t>Lvl 90 Mage</t>
-  </si>
-  <si>
     <t>Armour balaala</t>
   </si>
   <si>
@@ -86,18 +71,12 @@
     <t>Pieces</t>
   </si>
   <si>
-    <t>Ammount</t>
-  </si>
-  <si>
     <t>Character</t>
   </si>
   <si>
     <t>Points</t>
   </si>
   <si>
-    <t>ProductID</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -116,16 +95,103 @@
     <t>Product Types</t>
   </si>
   <si>
-    <t>Product Type</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
     <t>Attribute</t>
   </si>
   <si>
-    <t>TypeID</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>VendorId</t>
+  </si>
+  <si>
+    <t>MeasureId</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>DetailsId</t>
+  </si>
+  <si>
+    <t>Bars</t>
+  </si>
+  <si>
+    <t>Thronium</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>Base Prise</t>
+  </si>
+  <si>
+    <t>SubType</t>
+  </si>
+  <si>
+    <t>Two handed sword</t>
+  </si>
+  <si>
+    <t>Forged in the deep mountains of Azeroth …</t>
+  </si>
+  <si>
+    <t>CharacterNameHere</t>
+  </si>
+  <si>
+    <t>Horde</t>
+  </si>
+  <si>
+    <t>Lvl 90 Mage Rating 985 Gearscore 1293</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>Ore</t>
+  </si>
+  <si>
+    <t>Thronium is mined from the deepest ….</t>
+  </si>
+  <si>
+    <t>This sales report will be translated to this sales object in MS SQL</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>DateId</t>
+  </si>
+  <si>
+    <t>SaleDate</t>
+  </si>
+  <si>
+    <t>SellerName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SellerId</t>
   </si>
 </sst>
 </file>
@@ -177,7 +243,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +274,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -363,12 +447,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -385,9 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,6 +536,12 @@
     <xf numFmtId="2" fontId="5" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -442,9 +560,45 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,7 +695,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -726,80 +880,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="18" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="37">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
         <v>15.99</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4">
         <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -807,39 +970,45 @@
       <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="37">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
         <v>299.99</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="37">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
         <v>34.99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
         <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -847,19 +1016,22 @@
       <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="37">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4">
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
@@ -867,215 +1039,435 @@
       <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="37">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+    <row r="8" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="37">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="D10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="B17" s="22"/>
+      <c r="D17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="D18" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="33">
+        <v>1</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>2</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="B20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="33">
+        <v>2</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>3</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="8">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="D21" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="33">
+        <v>6</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>5</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>4</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="8">
-        <v>3</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="C26" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="D26" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>2</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>3</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <v>1</v>
-      </c>
-      <c r="B25" s="10">
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
         <v>90</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C27" s="9">
         <v>19.989999999999998</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D27" s="10">
         <f>19.99*90</f>
         <v>1799.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="E27" s="30"/>
+      <c r="F27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
         <v>4</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B28" s="9">
         <v>10000</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C28" s="9">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D28" s="10">
         <f>10000*1.09</f>
         <v>10900</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+      <c r="E28" s="30"/>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>90</v>
+      </c>
+      <c r="I28">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="J28" s="42">
+        <v>1</v>
+      </c>
+      <c r="K28" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <v>3</v>
       </c>
-      <c r="B27" s="10">
-        <v>1</v>
-      </c>
-      <c r="C27" s="10">
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
         <v>42.49</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D29" s="10">
         <v>42.49</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="E29" s="30"/>
+      <c r="F29" s="5">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>10000</v>
+      </c>
+      <c r="I29">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J29" s="42">
+        <v>1</v>
+      </c>
+      <c r="K29" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="17">
+        <f>D27+D28+D29</f>
+        <v>12741.59</v>
+      </c>
+      <c r="E30" s="30"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F32" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="K32" s="38"/>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F33" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="18">
-        <f>D25+D26+D27</f>
-        <v>12741.59</v>
-      </c>
+      <c r="G33" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="39"/>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F34" s="40">
+        <v>1</v>
+      </c>
+      <c r="G34" s="41">
+        <v>36120</v>
+      </c>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39">
+        <v>1</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A23:D23"/>
+  <mergeCells count="9">
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A25:D25"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="E25:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>